<commit_message>
Updated database and export file
</commit_message>
<xml_diff>
--- a/weather_data_export.xlsx
+++ b/weather_data_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,26 +472,251 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>776</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>776</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>776</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>776</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>776</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>776</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>776</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
-        <v>776</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>СВ</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="B9" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>776</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>776</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>776</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Background work is separate
</commit_message>
<xml_diff>
--- a/weather_data_export.xlsx
+++ b/weather_data_export.xlsx
@@ -472,20 +472,20 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
         <v>776</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>С</t>
+          <t>В</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -497,20 +497,20 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
         <v>776</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>С</t>
+          <t>В</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -522,7 +522,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B4" t="n">
         <v>6</v>
@@ -531,11 +531,11 @@
         <v>776</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>С</t>
+          <t>СВ</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -547,7 +547,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B5" t="n">
         <v>6</v>
@@ -556,11 +556,11 @@
         <v>776</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>С</t>
+          <t>СВ</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -572,7 +572,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B6" t="n">
         <v>6</v>
@@ -581,11 +581,11 @@
         <v>776</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>С</t>
+          <t>СВ</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -597,7 +597,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -606,11 +606,11 @@
         <v>776</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>С</t>
+          <t>СВ</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -622,10 +622,10 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" t="n">
         <v>776</v>
@@ -647,10 +647,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="n">
         <v>776</v>
@@ -672,10 +672,10 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" t="n">
         <v>776</v>
@@ -697,10 +697,10 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" t="n">
         <v>776</v>

</xml_diff>